<commit_message>
revise according to the code review and update db schema
</commit_message>
<xml_diff>
--- a/management_app/static/data_templates/scheduled_teaching.xlsx
+++ b/management_app/static/data_templates/scheduled_teaching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/che/Desktop/mac_desktop/studyabroad/CS_learning/MSWE_course/Q5/03-276P_Capstone_Project/TeachingManagementWebApplication/management_app/static/data_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CA9F29-7055-9A49-BD95-C9C69117E054}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A39991D-FA85-8142-BF9B-15E63960B5DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,8 +512,8 @@
   </sheetPr>
   <dimension ref="A1:J991"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3688,7 +3688,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView zoomScale="171" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3746,5 +3746,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>